<commit_message>
suppression draft pour les scenarios OK en 3.2 et adaptations suite à MEP ROR (#367)
* mise a jour etiquette draft

ajout/suppr draft + stu-note

* Update consignes_fiche_saisie_offre.md

* Update consignes_fiche_saisie_offre.md

* adaptation capability statement apres MEP ROR

adaptation capability statement pa rapport à ce qui n'a pas été implémenté dans le ROR 3.2 mis en prod 235c333e3abc853f76034659265a4a45393edff9
</commit_message>
<xml_diff>
--- a/main/ig/ValueSet-act-type-ror-valueset.xlsx
+++ b/main/ig/ValueSet-act-type-ror-valueset.xlsx
@@ -7,7 +7,7 @@
   </bookViews>
   <sheets>
     <sheet name="Metadata" r:id="rId3" sheetId="1"/>
-    <sheet name="Include from ActTypeRORCodeSy" r:id="rId4" sheetId="2"/>
+    <sheet name="Include #0" r:id="rId4" sheetId="2"/>
   </sheets>
 </workbook>
 </file>
@@ -57,7 +57,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2024-07-09T14:18:56+00:00</t>
+    <t>2024-09-13T14:28:16+00:00</t>
   </si>
   <si>
     <t>Publisher</t>

</xml_diff>